<commit_message>
complete sprint 2 report
</commit_message>
<xml_diff>
--- a/sprint-backlog/sprint-2/report-sheet.xlsx
+++ b/sprint-backlog/sprint-2/report-sheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE33A427-9797-4458-AC26-9313A17D113A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457762AD-2406-4820-A1EF-06AB47ACC9F7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="25">
   <si>
     <t>Dependency</t>
   </si>
@@ -36,21 +36,12 @@
     <t>J:1</t>
   </si>
   <si>
-    <t>1: 10-26-2018</t>
-  </si>
-  <si>
-    <t>5: 10-22-2018</t>
-  </si>
-  <si>
     <t>K:1</t>
   </si>
   <si>
     <t>C:1</t>
   </si>
   <si>
-    <t>Z:1</t>
-  </si>
-  <si>
     <t>Z:3</t>
   </si>
   <si>
@@ -66,9 +57,6 @@
     <t>User Story</t>
   </si>
   <si>
-    <t>Task</t>
-  </si>
-  <si>
     <t>K:3</t>
   </si>
   <si>
@@ -93,13 +81,22 @@
     <t>C:2</t>
   </si>
   <si>
-    <t>T11</t>
-  </si>
-  <si>
     <t>1: 10-23-2018</t>
   </si>
   <si>
     <t>5: 10-27-2018</t>
+  </si>
+  <si>
+    <t>J:2</t>
+  </si>
+  <si>
+    <t>J:5</t>
+  </si>
+  <si>
+    <t>A:5</t>
+  </si>
+  <si>
+    <t>C:3</t>
   </si>
 </sst>
 </file>
@@ -191,6 +188,14 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-CA"/>
+              <a:t>Sprint 2:</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA"/>
               <a:t>Burndown Chart Provisional vs Actual</a:t>
             </a:r>
           </a:p>
@@ -273,13 +278,13 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -328,6 +333,21 @@
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1633,10 +1653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" activeCellId="4" sqref="D2 D3 D4 D5 D7"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1646,10 +1666,10 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1658,7 +1678,7 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F1">
         <v>2</v>
@@ -1670,7 +1690,7 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1699,7 +1719,7 @@
         <v>3</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1713,19 +1733,19 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1739,13 +1759,13 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1759,13 +1779,13 @@
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1776,36 +1796,19 @@
         <v>11</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7">
-        <v>5</v>
-      </c>
-      <c r="G7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1815,20 +1818,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EF6B04-6D91-4CB2-B795-853A8560DA04}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1837,7 +1840,7 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="F1">
         <v>2</v>
@@ -1849,7 +1852,7 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1869,7 +1872,7 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
@@ -1878,7 +1881,7 @@
         <v>3</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1892,19 +1895,19 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1917,14 +1920,8 @@
       <c r="D4">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
       <c r="I4" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1938,13 +1935,16 @@
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>5</v>
       </c>
       <c r="I5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1955,36 +1955,19 @@
         <v>11</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7">
-        <v>5</v>
-      </c>
-      <c r="G7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1997,14 +1980,14 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -2027,7 +2010,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>40</v>
@@ -2036,13 +2019,13 @@
         <v>40</v>
       </c>
       <c r="D2">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E2">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F2">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -2050,10 +2033,25 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>40</v>
+      </c>
+      <c r="C3">
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <v>40</v>
+      </c>
+      <c r="E3">
+        <v>40</v>
+      </c>
+      <c r="F3">
+        <v>40</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed minor typo in burndown graph
</commit_message>
<xml_diff>
--- a/sprint-backlog/sprint-2/report-sheet.xlsx
+++ b/sprint-backlog/sprint-2/report-sheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457762AD-2406-4820-A1EF-06AB47ACC9F7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184B7209-18CC-4114-8E80-4BC036C770FF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="plan" sheetId="1" r:id="rId1"/>
@@ -66,9 +66,6 @@
     <t>day</t>
   </si>
   <si>
-    <t>acutal</t>
-  </si>
-  <si>
     <t>Tasks</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>C:3</t>
+  </si>
+  <si>
+    <t>actual</t>
   </si>
 </sst>
 </file>
@@ -308,7 +308,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>acutal</c:v>
+                  <c:v>actual</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1659,17 +1659,17 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1678,7 +1678,7 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F1">
         <v>2</v>
@@ -1690,10 +1690,10 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1719,10 +1719,10 @@
         <v>3</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1779,16 +1779,16 @@
         <v>8</v>
       </c>
       <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
         <v>17</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
       </c>
       <c r="I5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1824,14 +1824,14 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1840,7 +1840,7 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F1">
         <v>2</v>
@@ -1852,10 +1852,10 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
@@ -1881,10 +1881,10 @@
         <v>3</v>
       </c>
       <c r="I2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1921,10 +1921,10 @@
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G5" t="s">
         <v>5</v>
@@ -1947,7 +1947,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1979,13 +1979,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D36948-1878-4E62-8F83-9D21899FB0AC}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -2008,7 +2006,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2031,9 +2029,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <v>40</v>

</xml_diff>